<commit_message>
apply new customKeyword: waitForElementSpinnersNotPresent
</commit_message>
<xml_diff>
--- a/Data Files/searchResult.xlsx
+++ b/Data Files/searchResult.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="229">
   <si>
     <t/>
   </si>
@@ -20,688 +20,685 @@
     <t>Page_1</t>
   </si>
   <si>
+    <t>LOGITECH Keyboard USB K120 Classic Keyboard K120</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120</t>
+  </si>
+  <si>
+    <t>KEYBOARD USB LOGITECH K120</t>
+  </si>
+  <si>
+    <t>Keyboard LOGITECH K120 Usb ( Garansi Resmi )</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120</t>
+  </si>
+  <si>
+    <t>Logitech Keyboard K120</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Wired Full-Size Hitam Berkabel Universal Plug</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>Keyboard K120 Logitech K120 USB Wired Keyboard</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K100/KEYBOARD MURAH LOGITECH</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Wired</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Keyboard logitech K120</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>LOGITECH KEYBOARD K120 ORIGINAL</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Keyboard Komputer Eksternal Notbook Laptop Keyboard Logitech K100 PS2</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB - Hitam Original Garansi Resmi</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Logitech Classic keyboard K120 Black USB</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>keyboard Logitech K120 Produk 100% original, resmi Logitech,Murah</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Keyboard Kabel USB Logitech K120 Original by MegaPC</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Plug and Play USB Keyboard</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Logitech K120 Corded Keyboard</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Page_2</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Original Garansi Resmi</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 100% ORIGINAL / KEYBOARD USB PC LOGITECH ORIGINAL</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120 / KEYBOARD WIRED K120 / USB KEYBOARD K120</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Logitech USB Keyboard - K120</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech USB K120</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>KEYBOARD USB LOGITECH K120 [GARANSI RESMI]</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>KEYBOARD CLASSIC LOGITECH K120 / KEYBOARD LOGITECH K120</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Logitech K120 Wired USB Keyboard - Black</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 Original 100% Garansi Resmi 1 Tahun</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 Original - Garansi Resmi 1 Tahun</t>
+  </si>
+  <si>
+    <t>logitech keyboard k120 usb</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB</t>
+  </si>
+  <si>
+    <t>LOGITECH Keyboard Usb K120 Original</t>
+  </si>
+  <si>
+    <t>Keyboard USB Wired Logitech K120 Plug and Play</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech USB Kabel K-120 Logitech K120</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K100/KEYBOARD PC/KERBOARD LOGITECH</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Keyboard mouse LOGITECH WIRELESS K270 BEKAS ORIGINAL</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Usb Wired Keyboard</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Garansi resmi</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>Logitech K120 USB Wired Keyboard Original</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>Page_3</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120 USB ORIGINAL BANDUNG</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120 ORIGINAL</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech USB K120 Original Resmi</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Usb - Logitech K 120 Usb Keyboard</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K 120</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>USB Keyboard Logitech K120 Wired For Laptop Notebook Komputer PC</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Key board USB Komputer PC CPU Laptop</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>LOGITECH Keyboard USB K120 - 100% original</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 100% ORIGINAL</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Kabel USB Komputer PC Laptop Notebook</t>
+  </si>
+  <si>
+    <t>LOGITECH Keyboard USB K120</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Keyboard USB Original 100% PREMIUM STOCK</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Kabel Laptop PC Komputer Notebook</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Keyboard Usb Logitech k 120 original</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Keyboard USB Original 100%</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>LOGITECH CABLE KEYBOARD K120 USB / KEYBOARD K 120 ORIGINAL</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>keyboard logitech k120 usb original</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>Keyboard LOGITECH ASLI K120/Key Board Kabel LOGITECH/Keyboard USB K120</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>keyboard logitech USB K120 baru dan bergaransi resmi logitech dengan kabel USB</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>Logitech keyboard K120 USB / Keyboard Logitech Original / Logitech K120 USB / Keyboard</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Wired</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB - Hitam Garansi Resmi</t>
+  </si>
+  <si>
+    <t>Logitech K 100 Classic Keyboard - Hitam</t>
+  </si>
+  <si>
+    <t>Logitech K120 USB Keyboard</t>
+  </si>
+  <si>
+    <t>Keyboard Usb Logitech K120</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Kabel ORIGINAL</t>
+  </si>
+  <si>
+    <t>Keyboard LOGITECH K120 USB Kabel-Hitam</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>Keyboard USB LOGITECH K120 - 100% original</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 - Original</t>
+  </si>
+  <si>
+    <t>Keyboard usb Logitech K120 murah</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 Original Garansi 1 Tahun</t>
+  </si>
+  <si>
+    <t>Logitech keyboard k120 usb original</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB - Black</t>
+  </si>
+  <si>
+    <t>Keyboard USB - Logitech K120 GARANSI RESMI MURAH</t>
+  </si>
+  <si>
+    <t>KEYBOARD KETIK KOMPUTER - LOGITECH K120 GARANSI RESMI</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech Murah K120 - Corded Keyboard Plug And Play - Keybaoard PC &amp; Laptop</t>
+  </si>
+  <si>
+    <t>KEYBOARD USB LOGITECH K120 / KEYBOARD BERKABEL / KEYBOARD UNTUK PC DAN LAPTOP</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120 USB ORIGINAL</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH K120 USB</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Logitech USB Keyboard - K120 - Hitam K 120 plug and play wayar wired cable kabel berkabel pc cpu laptop komputer rakit rakitan AIO</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 - ORI Garansi Resmi 3th</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH USB K120</t>
+  </si>
+  <si>
+    <t>ITAcc Logitech Keyboard USB K120 - Hitam</t>
+  </si>
+  <si>
+    <t>Logitech K120 Corded Keyboard USB Plug-and-Play - Garansi Resmi 1 Tahun</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Original</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB wired Original Resmi</t>
+  </si>
+  <si>
+    <t>keyboard logitech k120 / KEY11-LOG</t>
+  </si>
+  <si>
+    <t>Logitech USB Keyboard - K120 - Black</t>
+  </si>
+  <si>
+    <t>Logitech Keyboard K120 USB Wired Plug and Play Garansi Resmi</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB Wired Keyboard Original</t>
+  </si>
+  <si>
+    <t>Keyboard Kabel USB K120 - Logitech</t>
+  </si>
+  <si>
+    <t>Keyboard USB Logitech K120 USB Original Resmi</t>
+  </si>
+  <si>
+    <t>FAK - Logitech K120 / K-120 Keyboard USB - Hitam</t>
+  </si>
+  <si>
+    <t>Keyboard Logitech K120 USB KABEL Wire ORIGINAL</t>
+  </si>
+  <si>
+    <t>Logitech Keyboard USB K120 - Hitam</t>
+  </si>
+  <si>
+    <t>LOGITECH KEYBOARD K120</t>
+  </si>
+  <si>
     <t>Keyboard USB LOGITECH K120 Keyboard Komputer Keyboard Laptop</t>
   </si>
   <si>
+    <t>Keyboard logitech wired usb 2.0 standard classic membrane silent K120 K-120 original</t>
+  </si>
+  <si>
+    <t>KEYBOARD LOGITECH USB K-120 ORIGINAL-DISASS JOGJA</t>
+  </si>
+  <si>
+    <t>Keyboard logitech wired usb 2.0 standard classic membrane silent K-120 K120 original</t>
+  </si>
+  <si>
     <t>KEYBOARD USB LOGITECH ORIGINAL K120</t>
-  </si>
-  <si>
-    <t>LOGITECH Keyboard USB K120 Classic Keyboard K120</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120</t>
-  </si>
-  <si>
-    <t>KEYBOARD USB LOGITECH K120</t>
-  </si>
-  <si>
-    <t>Keyboard LOGITECH K120 Usb ( Garansi Resmi )</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K120</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>Logitech Keyboard K120</t>
-  </si>
-  <si>
-    <t>108</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>Keyboard K120 Logitech K120 USB Wired Keyboard</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K100/KEYBOARD MURAH LOGITECH</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Wired Full-Size Hitam Berkabel Universal Plug</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Wired</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Keyboard logitech K120</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>LOGITECH KEYBOARD K120 ORIGINAL</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Keyboard Komputer Eksternal Notbook Laptop Keyboard Logitech K100 PS2</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB - Hitam Original Garansi Resmi</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Logitech Classic keyboard K120 Black USB</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>Keyboard Kabel USB Logitech K120 Original by MegaPC</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>keyboard Logitech K120 Produk 100% original, resmi Logitech,Murah</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Page_2</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Plug and Play USB Keyboard</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Logitech K120 Corded Keyboard</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Original Garansi Resmi</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 100% ORIGINAL / KEYBOARD USB PC LOGITECH ORIGINAL</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K120 / KEYBOARD WIRED K120 / USB KEYBOARD K120</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Logitech USB Keyboard - K120</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>KEYBOARD USB LOGITECH K120 [GARANSI RESMI]</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Logitech K120 Wired USB Keyboard - Black</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
-    <t>Logitech H111 Headset Stereo dengan Headband Adjustable dan Single Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 Original 100% Garansi Resmi 1 Tahun</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 Original - Garansi Resmi 1 Tahun</t>
-  </si>
-  <si>
-    <t>logitech keyboard k120 usb</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB</t>
-  </si>
-  <si>
-    <t>LOGITECH Keyboard Usb K120 Original</t>
-  </si>
-  <si>
-    <t>KEYBOARD CLASSIC LOGITECH K120 / KEYBOARD LOGITECH K120</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech USB K120</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech USB Kabel K-120 Logitech K120</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>Keyboard mouse LOGITECH WIRELESS K270 BEKAS ORIGINAL</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>NYK Nemesis Eris K06 Keyboard Gaming 61% with Holder</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K100/KEYBOARD PC/KERBOARD LOGITECH</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Usb Wired Keyboard</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>Page_3</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Garansi resmi</t>
-  </si>
-  <si>
-    <t>39</t>
-  </si>
-  <si>
-    <t>Logitech K120 USB Wired Keyboard Original</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech USB K120 Original Resmi</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K120 USB ORIGINAL BANDUNG</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Usb - Logitech K 120 Usb Keyboard</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K120 ORIGINAL</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>USB Keyboard Logitech K120 Wired For Laptop Notebook Komputer PC</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>46</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K 120</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Key board USB Komputer PC CPU Laptop</t>
-  </si>
-  <si>
-    <t>LOGITECH Keyboard USB K120 - 100% original</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t>LOGITECH Keyboard USB K120</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 100% ORIGINAL</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Kabel Laptop PC Komputer Notebook</t>
-  </si>
-  <si>
-    <t>52</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Kabel USB Komputer PC Laptop Notebook</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Keyboard USB Original 100%</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Keyboard USB Original 100% PREMIUM STOCK</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>keyboard logitech k120 usb original</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>Keyboard Usb Logitech k 120 original</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>Logitech K 100 Classic Keyboard - Hitam</t>
-  </si>
-  <si>
-    <t>Logitech K120 USB Keyboard</t>
-  </si>
-  <si>
-    <t>Keyboard Usb Logitech K120</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Kabel ORIGINAL</t>
-  </si>
-  <si>
-    <t>Keyboard LOGITECH K120 USB Kabel-Hitam</t>
-  </si>
-  <si>
-    <t>Keyboard LOGITECH ASLI K120/Key Board Kabel LOGITECH/Keyboard USB K120</t>
-  </si>
-  <si>
-    <t>keyboard logitech USB K120 baru dan bergaransi resmi logitech dengan kabel USB</t>
-  </si>
-  <si>
-    <t>LOGITECH CABLE KEYBOARD K120 USB / KEYBOARD K 120 ORIGINAL</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>76</t>
-  </si>
-  <si>
-    <t>77</t>
-  </si>
-  <si>
-    <t>78</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 Original Garansi 1 Tahun</t>
-  </si>
-  <si>
-    <t>Logitech keyboard k120 usb original</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB - Black</t>
-  </si>
-  <si>
-    <t>Keyboard USB - Logitech K120 GARANSI RESMI MURAH</t>
-  </si>
-  <si>
-    <t>KEYBOARD KETIK KOMPUTER - LOGITECH K120 GARANSI RESMI</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech Murah K120 - Corded Keyboard Plug And Play - Keybaoard PC &amp; Laptop</t>
-  </si>
-  <si>
-    <t>KEYBOARD USB LOGITECH K120 / KEYBOARD BERKABEL / KEYBOARD UNTUK PC DAN LAPTOP</t>
-  </si>
-  <si>
-    <t>Logitech keyboard K120 USB / Keyboard Logitech Original / Logitech K120 USB / Keyboard</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Wired</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB - Hitam Garansi Resmi</t>
-  </si>
-  <si>
-    <t>79</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 - Original</t>
-  </si>
-  <si>
-    <t>Keyboard usb Logitech K120 murah</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 - ORI Garansi Resmi 3th</t>
-  </si>
-  <si>
-    <t>Keyboard USB Wired Logitech K120 Plug and Play</t>
-  </si>
-  <si>
-    <t>ITAcc Logitech Keyboard USB K120 - Hitam</t>
-  </si>
-  <si>
-    <t>Logitech USB Keyboard - K120 - Hitam K 120 plug and play wayar wired cable kabel berkabel pc cpu laptop komputer rakit rakitan AIO</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Original</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH USB K120</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB wired Original Resmi</t>
-  </si>
-  <si>
-    <t>Logitech K120 Corded Keyboard USB Plug-and-Play - Garansi Resmi 1 Tahun</t>
-  </si>
-  <si>
-    <t>Logitech USB Keyboard - K120 - Black</t>
-  </si>
-  <si>
-    <t>keyboard logitech k120 / KEY11-LOG</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB Wired Keyboard Original</t>
-  </si>
-  <si>
-    <t>Logitech Keyboard K120 USB Wired Plug and Play Garansi Resmi</t>
-  </si>
-  <si>
-    <t>FAK - Logitech Keyboard Standar PS2 K100 atau USB K120 - Hitam</t>
-  </si>
-  <si>
-    <t>Keyboard Kabel USB K120 - Logitech</t>
-  </si>
-  <si>
-    <t>Keyboard USB Logitech K120 USB Original Resmi</t>
-  </si>
-  <si>
-    <t>Keyboard Logitech K120 USB KABEL Wire ORIGINAL</t>
-  </si>
-  <si>
-    <t>FAK - Logitech K120 / K-120 Keyboard USB - Hitam</t>
-  </si>
-  <si>
-    <t>Logitech Keyboard USB K120 - Hitam</t>
-  </si>
-  <si>
-    <t>LOGITECH KEYBOARD K120</t>
-  </si>
-  <si>
-    <t>Keyboard logitech wired usb 2.0 standard classic membrane silent K120 K-120 original</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH USB K-120 ORIGINAL-DISASS JOGJA</t>
-  </si>
-  <si>
-    <t>Keyboard logitech wired usb 2.0 standard classic membrane silent K-120 K120 original</t>
-  </si>
-  <si>
-    <t>KEYBOARD LOGITECH K120 USB</t>
   </si>
 </sst>
 </file>
@@ -771,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -925,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17">
@@ -936,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18">
@@ -947,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19">
@@ -958,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20">
@@ -969,7 +966,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>216</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
@@ -980,7 +977,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22">
@@ -991,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23">
@@ -1002,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24">
@@ -1013,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>218</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -1024,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26">
@@ -1035,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27">
@@ -1046,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>221</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -1057,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29">
@@ -1068,18 +1065,18 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>37</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31">
@@ -1101,34 +1098,34 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
@@ -1139,7 +1136,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -1150,35 +1147,35 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>226</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>228</v>
       </c>
     </row>
     <row r="40">
@@ -1189,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41">
@@ -1205,7 +1202,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
         <v>65</v>
@@ -1216,7 +1213,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B43" t="s">
         <v>65</v>
@@ -1227,7 +1224,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
@@ -1238,7 +1235,7 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
@@ -1249,7 +1246,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B46" t="s">
         <v>65</v>
@@ -1409,7 +1406,7 @@
         <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61">
@@ -1431,7 +1428,7 @@
         <v>65</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63">
@@ -1519,7 +1516,7 @@
         <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71">
@@ -1530,7 +1527,7 @@
         <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="72">
@@ -1552,7 +1549,7 @@
         <v>65</v>
       </c>
       <c r="C73" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74">
@@ -1563,7 +1560,7 @@
         <v>65</v>
       </c>
       <c r="C74" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75">
@@ -1574,7 +1571,7 @@
         <v>65</v>
       </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="76">
@@ -1585,7 +1582,7 @@
         <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77">
@@ -1596,7 +1593,7 @@
         <v>65</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78">
@@ -1607,7 +1604,7 @@
         <v>65</v>
       </c>
       <c r="C78" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79">
@@ -1618,7 +1615,7 @@
         <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="80">
@@ -1629,7 +1626,7 @@
         <v>65</v>
       </c>
       <c r="C80" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81">
@@ -1648,7 +1645,7 @@
         <v>187</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C82" t="s">
         <v>109</v>
@@ -1659,10 +1656,10 @@
         <v>188</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84">
@@ -1670,10 +1667,10 @@
         <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
     </row>
     <row r="85">
@@ -1681,10 +1678,10 @@
         <v>190</v>
       </c>
       <c r="B85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86">
@@ -1692,10 +1689,10 @@
         <v>191</v>
       </c>
       <c r="B86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87">
@@ -1703,10 +1700,10 @@
         <v>192</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C87" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88">
@@ -1714,10 +1711,10 @@
         <v>193</v>
       </c>
       <c r="B88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="89">
@@ -1725,7 +1722,7 @@
         <v>194</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C89" t="s">
         <v>125</v>
@@ -1736,7 +1733,7 @@
         <v>197</v>
       </c>
       <c r="B90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C90" t="s">
         <v>128</v>
@@ -1747,7 +1744,7 @@
         <v>198</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C91" t="s">
         <v>127</v>
@@ -1758,7 +1755,7 @@
         <v>199</v>
       </c>
       <c r="B92" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C92" t="s">
         <v>132</v>
@@ -1769,7 +1766,7 @@
         <v>200</v>
       </c>
       <c r="B93" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
         <v>130</v>
@@ -1780,7 +1777,7 @@
         <v>201</v>
       </c>
       <c r="B94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
         <v>136</v>
@@ -1791,7 +1788,7 @@
         <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C95" t="s">
         <v>134</v>
@@ -1802,7 +1799,7 @@
         <v>203</v>
       </c>
       <c r="B96" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C96" t="s">
         <v>140</v>
@@ -1813,7 +1810,7 @@
         <v>204</v>
       </c>
       <c r="B97" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C97" t="s">
         <v>138</v>
@@ -1824,7 +1821,7 @@
         <v>205</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C98" t="s">
         <v>144</v>
@@ -1835,7 +1832,7 @@
         <v>206</v>
       </c>
       <c r="B99" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99" t="s">
         <v>142</v>
@@ -1846,7 +1843,7 @@
         <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C100" t="s">
         <v>164</v>
@@ -1857,10 +1854,10 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C101" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
     </row>
     <row r="102">
@@ -1868,10 +1865,10 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C102" t="s">
-        <v>162</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103">
@@ -1879,10 +1876,10 @@
         <v>18</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="104">
@@ -1890,10 +1887,10 @@
         <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C104" t="s">
-        <v>37</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105">
@@ -1901,10 +1898,10 @@
         <v>16</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C105" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106">
@@ -1912,7 +1909,7 @@
         <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C106" t="s">
         <v>160</v>
@@ -1923,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="B107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C107" t="s">
         <v>159</v>
@@ -1934,7 +1931,7 @@
         <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C108" t="s">
         <v>158</v>
@@ -1945,7 +1942,7 @@
         <v>11</v>
       </c>
       <c r="B109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C109" t="s">
         <v>157</v>
@@ -1956,7 +1953,7 @@
         <v>60</v>
       </c>
       <c r="B110" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
         <v>184</v>
@@ -1967,7 +1964,7 @@
         <v>57</v>
       </c>
       <c r="B111" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C111" t="s">
         <v>183</v>
@@ -1978,7 +1975,7 @@
         <v>58</v>
       </c>
       <c r="B112" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C112" t="s">
         <v>182</v>
@@ -1989,7 +1986,7 @@
         <v>55</v>
       </c>
       <c r="B113" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C113" t="s">
         <v>181</v>
@@ -2000,7 +1997,7 @@
         <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
         <v>180</v>
@@ -2011,7 +2008,7 @@
         <v>53</v>
       </c>
       <c r="B115" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C115" t="s">
         <v>179</v>
@@ -2022,7 +2019,7 @@
         <v>54</v>
       </c>
       <c r="B116" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C116" t="s">
         <v>178</v>
@@ -2033,7 +2030,7 @@
         <v>50</v>
       </c>
       <c r="B117" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C117" t="s">
         <v>177</v>
@@ -2044,7 +2041,7 @@
         <v>52</v>
       </c>
       <c r="B118" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C118" t="s">
         <v>176</v>
@@ -2055,7 +2052,7 @@
         <v>46</v>
       </c>
       <c r="B119" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C119" t="s">
         <v>175</v>
@@ -2066,7 +2063,7 @@
         <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C120" t="s">
         <v>196</v>
@@ -2077,7 +2074,7 @@
         <v>85</v>
       </c>
       <c r="B121" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C121" t="s">
         <v>195</v>

</xml_diff>